<commit_message>
훈련대상 API - import, export 수정보완
</commit_message>
<xml_diff>
--- a/Spreadsheet/Target.xlsx
+++ b/Spreadsheet/Target.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taeho\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taeho\go\src\redteam\Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2364" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,71 +46,70 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>태그</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정된 시간(작성 X)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김태호</t>
+  </si>
+  <si>
+    <t>sjabber@naver.com</t>
+  </si>
+  <si>
+    <t>010-9856-1765</t>
+  </si>
+  <si>
+    <t>개발</t>
+  </si>
+  <si>
+    <t>신입</t>
+  </si>
+  <si>
+    <t>부분훈련</t>
+  </si>
+  <si>
     <t>홍길동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gildong@gmail.com</t>
+  </si>
+  <si>
+    <t>010-7575-1234</t>
+  </si>
+  <si>
+    <t>마케팅</t>
+  </si>
+  <si>
+    <t>과장</t>
+  </si>
+  <si>
+    <t>전체훈련</t>
   </si>
   <si>
     <t>루삥뽕</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sjabber@naver.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gildong@gmail.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ppingbbong@hanmail.net</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010-9856-1765</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010-7575-1234</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>010-1234-5678</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>개발</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마케팅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>인사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>신입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>대리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>과장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김태호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +143,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,7 +178,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -181,6 +189,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,23 +475,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.09765625" customWidth="1"/>
-    <col min="2" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="21.296875" customWidth="1"/>
-    <col min="5" max="5" width="21.59765625" customWidth="1"/>
-    <col min="6" max="6" width="19.796875" customWidth="1"/>
+    <col min="1" max="7" width="30.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -496,73 +502,76 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>